<commit_message>
Update Work Week and Social Spending
</commit_message>
<xml_diff>
--- a/www/IndicatorsPerCountry/Afghanistan_GDPperCapita_TerritorialRef_1946_2012_CCode_4.xlsx
+++ b/www/IndicatorsPerCountry/Afghanistan_GDPperCapita_TerritorialRef_1946_2012_CCode_4.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="82">
   <si>
     <t>Country Code</t>
   </si>
@@ -36,166 +36,193 @@
     <t>GDP per Capita</t>
   </si>
   <si>
-    <t>645</t>
-  </si>
-  <si>
-    <t>653</t>
-  </si>
-  <si>
-    <t>664</t>
-  </si>
-  <si>
-    <t>692</t>
-  </si>
-  <si>
-    <t>694</t>
-  </si>
-  <si>
-    <t>695</t>
-  </si>
-  <si>
-    <t>713</t>
-  </si>
-  <si>
-    <t>699</t>
-  </si>
-  <si>
-    <t>723</t>
-  </si>
-  <si>
-    <t>729</t>
-  </si>
-  <si>
-    <t>739</t>
-  </si>
-  <si>
-    <t>730</t>
-  </si>
-  <si>
-    <t>726</t>
-  </si>
-  <si>
-    <t>720</t>
-  </si>
-  <si>
-    <t>710</t>
-  </si>
-  <si>
-    <t>712</t>
-  </si>
-  <si>
-    <t>719</t>
-  </si>
-  <si>
-    <t>709</t>
-  </si>
-  <si>
-    <t>659</t>
-  </si>
-  <si>
-    <t>630</t>
-  </si>
-  <si>
-    <t>684</t>
-  </si>
-  <si>
-    <t>703</t>
-  </si>
-  <si>
-    <t>721</t>
-  </si>
-  <si>
-    <t>737</t>
-  </si>
-  <si>
-    <t>669</t>
-  </si>
-  <si>
-    <t>704</t>
-  </si>
-  <si>
-    <t>689</t>
-  </si>
-  <si>
-    <t>690</t>
-  </si>
-  <si>
-    <t>764</t>
-  </si>
-  <si>
-    <t>833</t>
-  </si>
-  <si>
-    <t>863</t>
-  </si>
-  <si>
-    <t>847</t>
-  </si>
-  <si>
-    <t>819</t>
-  </si>
-  <si>
-    <t>878</t>
-  </si>
-  <si>
-    <t>656</t>
-  </si>
-  <si>
-    <t>640</t>
-  </si>
-  <si>
-    <t>604</t>
-  </si>
-  <si>
-    <t>601</t>
-  </si>
-  <si>
-    <t>553</t>
-  </si>
-  <si>
-    <t>476</t>
-  </si>
-  <si>
-    <t>426</t>
-  </si>
-  <si>
-    <t>512</t>
-  </si>
-  <si>
-    <t>526</t>
-  </si>
-  <si>
-    <t>541</t>
-  </si>
-  <si>
-    <t>556</t>
-  </si>
-  <si>
-    <t>571</t>
-  </si>
-  <si>
-    <t>565</t>
-  </si>
-  <si>
-    <t>507</t>
-  </si>
-  <si>
-    <t>619</t>
-  </si>
-  <si>
-    <t>668</t>
-  </si>
-  <si>
-    <t>685</t>
-  </si>
-  <si>
-    <t>758</t>
-  </si>
-  <si>
-    <t>790</t>
-  </si>
-  <si>
-    <t>869</t>
+    <t>1156</t>
+  </si>
+  <si>
+    <t>1170</t>
+  </si>
+  <si>
+    <t>1189</t>
+  </si>
+  <si>
+    <t>1240</t>
+  </si>
+  <si>
+    <t>1245</t>
+  </si>
+  <si>
+    <t>1246</t>
+  </si>
+  <si>
+    <t>1278</t>
+  </si>
+  <si>
+    <t>1253</t>
+  </si>
+  <si>
+    <t>1298</t>
+  </si>
+  <si>
+    <t>1307</t>
+  </si>
+  <si>
+    <t>1326</t>
+  </si>
+  <si>
+    <t>1309</t>
+  </si>
+  <si>
+    <t>1302</t>
+  </si>
+  <si>
+    <t>1291</t>
+  </si>
+  <si>
+    <t>1290</t>
+  </si>
+  <si>
+    <t>1272</t>
+  </si>
+  <si>
+    <t>1277</t>
+  </si>
+  <si>
+    <t>1237</t>
+  </si>
+  <si>
+    <t>1007</t>
+  </si>
+  <si>
+    <t>1011</t>
+  </si>
+  <si>
+    <t>1039</t>
+  </si>
+  <si>
+    <t>1074</t>
+  </si>
+  <si>
+    <t>1105</t>
+  </si>
+  <si>
+    <t>1022</t>
+  </si>
+  <si>
+    <t>1070</t>
+  </si>
+  <si>
+    <t>1023</t>
+  </si>
+  <si>
+    <t>1019</t>
+  </si>
+  <si>
+    <t>1144</t>
+  </si>
+  <si>
+    <t>1270</t>
+  </si>
+  <si>
+    <t>1347</t>
+  </si>
+  <si>
+    <t>1337</t>
+  </si>
+  <si>
+    <t>1304</t>
+  </si>
+  <si>
+    <t>1344</t>
+  </si>
+  <si>
+    <t>1211</t>
+  </si>
+  <si>
+    <t>1101</t>
+  </si>
+  <si>
+    <t>999</t>
+  </si>
+  <si>
+    <t>963</t>
+  </si>
+  <si>
+    <t>881.170438588735</t>
+  </si>
+  <si>
+    <t>843.875348899883</t>
+  </si>
+  <si>
+    <t>578.402744031048</t>
+  </si>
+  <si>
+    <t>428.424558289543</t>
+  </si>
+  <si>
+    <t>632.940396261985</t>
+  </si>
+  <si>
+    <t>600.175264462535</t>
+  </si>
+  <si>
+    <t>570.598118955881</t>
+  </si>
+  <si>
+    <t>545.038752668709</t>
+  </si>
+  <si>
+    <t>518.657866732878</t>
+  </si>
+  <si>
+    <t>502.372745598633</t>
+  </si>
+  <si>
+    <t>489.681996907494</t>
+  </si>
+  <si>
+    <t>796.816563246003</t>
+  </si>
+  <si>
+    <t>842.805165479659</t>
+  </si>
+  <si>
+    <t>869.039272786813</t>
+  </si>
+  <si>
+    <t>964.4081099473</t>
+  </si>
+  <si>
+    <t>1057.09655092876</t>
+  </si>
+  <si>
+    <t>1259.99674275737</t>
+  </si>
+  <si>
+    <t>1319.60736728553</t>
+  </si>
+  <si>
+    <t>1557.32063657228</t>
+  </si>
+  <si>
+    <t>1627.67163410066</t>
+  </si>
+  <si>
+    <t>1792</t>
+  </si>
+  <si>
+    <t>1945</t>
+  </si>
+  <si>
+    <t>2025</t>
+  </si>
+  <si>
+    <t>2022</t>
+  </si>
+  <si>
+    <t>1928</t>
+  </si>
+  <si>
+    <t>1929</t>
   </si>
   <si>
     <t>Description</t>
@@ -568,7 +595,7 @@
         <v>1965.0</v>
       </c>
       <c r="E17" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18">
@@ -585,7 +612,7 @@
         <v>1966.0</v>
       </c>
       <c r="E18" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19">
@@ -602,7 +629,7 @@
         <v>1967.0</v>
       </c>
       <c r="E19" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20">
@@ -619,7 +646,7 @@
         <v>1968.0</v>
       </c>
       <c r="E20" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21">
@@ -653,7 +680,7 @@
         <v>1970.0</v>
       </c>
       <c r="E22" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23">
@@ -670,7 +697,7 @@
         <v>1971.0</v>
       </c>
       <c r="E23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24">
@@ -687,7 +714,7 @@
         <v>1972.0</v>
       </c>
       <c r="E24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25">
@@ -704,7 +731,7 @@
         <v>1973.0</v>
       </c>
       <c r="E25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26">
@@ -721,7 +748,7 @@
         <v>1974.0</v>
       </c>
       <c r="E26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="27">
@@ -738,7 +765,7 @@
         <v>1975.0</v>
       </c>
       <c r="E27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="28">
@@ -755,7 +782,7 @@
         <v>1976.0</v>
       </c>
       <c r="E28" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="29">
@@ -772,7 +799,7 @@
         <v>1977.0</v>
       </c>
       <c r="E29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="30">
@@ -789,7 +816,7 @@
         <v>1978.0</v>
       </c>
       <c r="E30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="31">
@@ -806,7 +833,7 @@
         <v>1979.0</v>
       </c>
       <c r="E31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="32">
@@ -823,7 +850,7 @@
         <v>1980.0</v>
       </c>
       <c r="E32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="33">
@@ -840,7 +867,7 @@
         <v>1981.0</v>
       </c>
       <c r="E33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="34">
@@ -857,7 +884,7 @@
         <v>1982.0</v>
       </c>
       <c r="E34" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="35">
@@ -874,7 +901,7 @@
         <v>1983.0</v>
       </c>
       <c r="E35" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="36">
@@ -891,7 +918,7 @@
         <v>1984.0</v>
       </c>
       <c r="E36" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="37">
@@ -908,7 +935,7 @@
         <v>1985.0</v>
       </c>
       <c r="E37" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="38">
@@ -925,7 +952,7 @@
         <v>1986.0</v>
       </c>
       <c r="E38" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="39">
@@ -942,7 +969,7 @@
         <v>1987.0</v>
       </c>
       <c r="E39" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
     </row>
     <row r="40">
@@ -1282,7 +1309,7 @@
         <v>2007.0</v>
       </c>
       <c r="E59" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
     </row>
     <row r="60">
@@ -1299,7 +1326,143 @@
         <v>2008.0</v>
       </c>
       <c r="E60" t="s">
-        <v>60</v>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B61" t="s">
+        <v>5</v>
+      </c>
+      <c r="C61" t="s">
+        <v>6</v>
+      </c>
+      <c r="D61" t="n">
+        <v>2009.0</v>
+      </c>
+      <c r="E61" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B62" t="s">
+        <v>5</v>
+      </c>
+      <c r="C62" t="s">
+        <v>6</v>
+      </c>
+      <c r="D62" t="n">
+        <v>2010.0</v>
+      </c>
+      <c r="E62" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B63" t="s">
+        <v>5</v>
+      </c>
+      <c r="C63" t="s">
+        <v>6</v>
+      </c>
+      <c r="D63" t="n">
+        <v>2011.0</v>
+      </c>
+      <c r="E63" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B64" t="s">
+        <v>5</v>
+      </c>
+      <c r="C64" t="s">
+        <v>6</v>
+      </c>
+      <c r="D64" t="n">
+        <v>2012.0</v>
+      </c>
+      <c r="E64" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B65" t="s">
+        <v>5</v>
+      </c>
+      <c r="C65" t="s">
+        <v>6</v>
+      </c>
+      <c r="D65" t="n">
+        <v>2013.0</v>
+      </c>
+      <c r="E65" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B66" t="s">
+        <v>5</v>
+      </c>
+      <c r="C66" t="s">
+        <v>6</v>
+      </c>
+      <c r="D66" t="n">
+        <v>2014.0</v>
+      </c>
+      <c r="E66" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B67" t="s">
+        <v>5</v>
+      </c>
+      <c r="C67" t="s">
+        <v>6</v>
+      </c>
+      <c r="D67" t="n">
+        <v>2015.0</v>
+      </c>
+      <c r="E67" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B68" t="s">
+        <v>5</v>
+      </c>
+      <c r="C68" t="s">
+        <v>6</v>
+      </c>
+      <c r="D68" t="n">
+        <v>2016.0</v>
+      </c>
+      <c r="E68" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1317,50 +1480,50 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B1" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="B2" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="B3" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="B4" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="B5" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="B6" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>